<commit_message>
cap nhat bidv qrcode
</commit_message>
<xml_diff>
--- a/BIDVQR/template.xlsx
+++ b/BIDVQR/template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\VietQR\VietQR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\VietQR-BIDV\BIDVQR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09032437-A161-42CD-9138-194868CA314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9735"/>
+    <workbookView xWindow="7200" yWindow="2010" windowWidth="21600" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Stt</t>
   </si>
@@ -34,14 +35,11 @@
   <si>
     <t>Tai_khoan</t>
   </si>
-  <si>
-    <t>ThuongHieu</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,30 +350,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cap nhat tentcard Bổ sung nôi dung cập nhật lại thư viện pdf to image
</commit_message>
<xml_diff>
--- a/BIDVQR/template.xlsx
+++ b/BIDVQR/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\VietQR-BIDV\BIDVQR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09032437-A161-42CD-9138-194868CA314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E428C-783C-46BE-B1CB-C0A9F2CE9811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2010" windowWidth="21600" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Stt</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Tai_khoan</t>
+  </si>
+  <si>
+    <t>Mo_ta</t>
   </si>
 </sst>
 </file>
@@ -351,18 +354,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,6 +376,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
thêm cn và cb liên hệ trên tempalte 2 trang
</commit_message>
<xml_diff>
--- a/BIDVQR/template.xlsx
+++ b/BIDVQR/template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\VietQR-BIDV\BIDVQR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\VietQR\BIDVQR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E428C-783C-46BE-B1CB-C0A9F2CE9811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Stt</t>
   </si>
@@ -37,12 +36,18 @@
   </si>
   <si>
     <t>Mo_ta</t>
+  </si>
+  <si>
+    <t>Chi_Nhanh</t>
+  </si>
+  <si>
+    <t>Can_Bo_Lien_He</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,20 +358,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G8" sqref="G8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,6 +385,12 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>